<commit_message>
Complete the leads assign
</commit_message>
<xml_diff>
--- a/Original_Data_Set.xlsx
+++ b/Original_Data_Set.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="124">
   <si>
     <t>File No.</t>
   </si>
@@ -390,6 +390,15 @@
   </si>
   <si>
     <t>Dharkast Road (Kishkindha Main Road), Kannadapalayam, West Tambaram, Chennai 600045, comprised in Old S.Nos.268/2, 268/3 &amp; 268/4, and T.S.Nos.106/1, 107/2, 107/3, 108/2 &amp; 108/3, Block No.21, Ward No.C of Tambaram Village, Tambaram Taluk within the Limits of Tambaram Municipal Corporation</t>
+  </si>
+  <si>
+    <t>9.P.Elanchezhiyan. B.Arch.,M.T.P</t>
+  </si>
+  <si>
+    <t>CMDA Regn. No. RA/Gr.I/19/06/276, No. 14/S2, Thirumurthy Nagar, Madananda puram,, Chennai- 600 125.</t>
+  </si>
+  <si>
+    <t>elan@rspindia.net</t>
   </si>
 </sst>
 </file>
@@ -402,7 +411,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,13 +428,6 @@
     <font>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -876,152 +878,155 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1369,10 +1374,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1501,13 +1506,13 @@
       <c r="M2" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1551,13 +1556,13 @@
       <c r="M3" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="S3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="T3" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1601,13 +1606,13 @@
       <c r="M4" t="s">
         <v>61</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="R4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="S4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1651,13 +1656,13 @@
       <c r="M5" t="s">
         <v>73</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="R5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="T5" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1701,13 +1706,13 @@
       <c r="M6" t="s">
         <v>86</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="R6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="S6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1751,13 +1756,13 @@
       <c r="M7" t="s">
         <v>98</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="R7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="S7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="T7" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1801,13 +1806,13 @@
       <c r="M8" t="s">
         <v>108</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="R8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="S8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="T8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1851,13 +1856,72 @@
       <c r="M9" t="s">
         <v>108</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="R9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="S9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" ht="15.75" spans="1:20">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="O10" t="s">
+        <v>122</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T10" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1887,6 +1951,9 @@
     <hyperlink ref="R9" r:id="rId22" display="View PDF"/>
     <hyperlink ref="S9" r:id="rId23" display="View Approved Plan"/>
     <hyperlink ref="T9" r:id="rId24" display="View Approval Letter"/>
+    <hyperlink ref="R10" r:id="rId1" display="View PDF"/>
+    <hyperlink ref="S10" r:id="rId2" display="View Approved Plan"/>
+    <hyperlink ref="T10" r:id="rId3" display="View Approval Letter"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
update the area names
</commit_message>
<xml_diff>
--- a/Original_Data_Set.xlsx
+++ b/Original_Data_Set.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t>File No.</t>
   </si>
@@ -89,40 +89,40 @@
     <t>Approval Letter</t>
   </si>
   <si>
-    <t>CMDA/PP/NHRB/S/0630/2024</t>
-  </si>
-  <si>
-    <t>OL-PP/NHRB/0025/2025</t>
-  </si>
-  <si>
-    <t>OL-01532</t>
-  </si>
-  <si>
-    <t>29-01-2025</t>
-  </si>
-  <si>
-    <t>11/09/2024</t>
-  </si>
-  <si>
-    <t>8754580801</t>
-  </si>
-  <si>
-    <t>athulyamenterprises@gmail.com</t>
-  </si>
-  <si>
-    <t>ATHULYAM ENTERPRISES PVT LTD Rep by Its Director Mr Krishnan</t>
-  </si>
-  <si>
-    <t>5/8, 1, Thiruveethi amman koil street, R A Puram, Mandaiveli, Adambakkam</t>
-  </si>
-  <si>
-    <t>Proposed construction of Stilt floor + 4 floors(Height - 15.25) Residential Building with 11 dwelling units Availing Premium FSI with TOD Benefit</t>
-  </si>
-  <si>
-    <t>11 dwelling units</t>
-  </si>
-  <si>
-    <t>Door No.5, Plot No.11, 5th street, Ram Nagar, Naganallur,Chennai-61 comprised in S.No.96/7 and T.S.No.34/2, Block No.15, Ward E of Adambakkam village within the limits of Greater Chennai Corporation</t>
+    <t>CMDA/PP/NHRB/S/0204/2025</t>
+  </si>
+  <si>
+    <t>OL-PP/NHRB/0239/2025</t>
+  </si>
+  <si>
+    <t>OL-01906</t>
+  </si>
+  <si>
+    <t>25-06-2025</t>
+  </si>
+  <si>
+    <t>22/03/2025</t>
+  </si>
+  <si>
+    <t>9444009349</t>
+  </si>
+  <si>
+    <t>venran2007@gmail.com</t>
+  </si>
+  <si>
+    <t>MS PRAGATHI PROPERTIES REP K VENKATESH</t>
+  </si>
+  <si>
+    <t>8/9, C 27, Chennai, THIRUVALLUR NAGAR ALANDUR, CHENNAI, Adambakkam</t>
+  </si>
+  <si>
+    <t>Planning Permission for the proposed construction of Stilt floor + 4 floors (Height - 15.0m) Residential Building with 8 dwelling units</t>
+  </si>
+  <si>
+    <t>8 dwelling units</t>
+  </si>
+  <si>
+    <t>Plot No.C-27, Door No.8/9, 1st Street, Thiruvalluvar Nagar, Alandur, Chennai 600016 comprised in Paimash No.861, 862 &amp; 863 (Document), Old S.No.27/2 and T.S.No.50, Block No.2, Ward - E (Patta) of Adambakkam Village, Alandur Taluk within the limits of Greater Chennai Corporation</t>
   </si>
   <si>
     <t>Adambakkam</t>
@@ -137,268 +137,196 @@
     <t>View Approval Letter</t>
   </si>
   <si>
-    <t>CMDA/PP/NHRB/N/0488/2025</t>
-  </si>
-  <si>
-    <t>OL-PP/NHRB/0349/2025</t>
-  </si>
-  <si>
-    <t>OL-02112</t>
-  </si>
-  <si>
-    <t>10-09-2025</t>
-  </si>
-  <si>
-    <t>23/06/2025</t>
-  </si>
-  <si>
-    <t>9840020301</t>
-  </si>
-  <si>
-    <t>vijayreva06@gmail.com</t>
-  </si>
-  <si>
-    <t>Ms India Builders Chennai Limited Represented by its Director Mr U Preetam Karthik AA36, AA36, 3rd</t>
-  </si>
-  <si>
-    <t>Street, 3rd Main Road, Anna Nagar, Koyambedu</t>
-  </si>
-  <si>
-    <t>Proposed construction of Stilt Floor + 5 Floors Residential building (18.30m Height) with 5 Dwelling units</t>
-  </si>
-  <si>
-    <t>5 Dwelling units</t>
-  </si>
-  <si>
-    <t>At Plot No.1368 Door No.4, 7th Street, Vallalar Kudiyurupu, Anna Nagar, Chennai 600 040 Comprised in S.No.154 pt, New S.No.154/2pt, T.S.No.73, Block No.37, I Block, Ward No.001, of Villivkkam Village within the limits of Greater Chennai Corporation</t>
+    <t>CMDA/PP/NHRB/S/0085/2025</t>
+  </si>
+  <si>
+    <t>OL-PP/NHRB/0218/2025</t>
+  </si>
+  <si>
+    <t>OL-01869</t>
+  </si>
+  <si>
+    <t>11-06-2025</t>
+  </si>
+  <si>
+    <t>06/02/2025</t>
+  </si>
+  <si>
+    <t>7092245303</t>
+  </si>
+  <si>
+    <t>aperiasamy@gmail.com</t>
+  </si>
+  <si>
+    <t>PERIASAMY ARNASALAM PILLAY AND P GEETHA</t>
+  </si>
+  <si>
+    <t>7, NIL, MARUTHAI AVENUE, OFF RANJITH ROAD, KOTTURPURAM, Adyar</t>
+  </si>
+  <si>
+    <t>Proposed construction of Stilt floor+ 3 floors Residential Building (Height-14.00 m) 6 Dwelling units</t>
+  </si>
+  <si>
+    <t>6 Dwelling units</t>
+  </si>
+  <si>
+    <t>Plot No.6 &amp; 103pt, Door No.7, Maruthai Avenue, Ranjith Cross Street, Kotturpuram, Chennai-600085 comprised in Old T.S.No 7 part and T.S.No.7/25 , 7/32, Block No.14 of Adyar Village within the limits of Greater Chennai Corporation</t>
   </si>
   <si>
     <t>Adyar</t>
   </si>
   <si>
-    <t>CMDA/PP/NHRB/C/0357/2025</t>
-  </si>
-  <si>
-    <t>OL-PP/NHRB/0294/2025</t>
-  </si>
-  <si>
-    <t>OL-01993</t>
-  </si>
-  <si>
-    <t>23-07-2025</t>
-  </si>
-  <si>
-    <t>19/05/2025</t>
-  </si>
-  <si>
-    <t>9483597940</t>
-  </si>
-  <si>
-    <t>landandbuildings@gmail.com</t>
-  </si>
-  <si>
-    <t>Ms Land and Buildings</t>
-  </si>
-  <si>
-    <t>Virugambakkam</t>
-  </si>
-  <si>
-    <t>Planning Permission Application for the proposed construction of Stilt floor + 4 floors (Height - 16.0m) Residential Building with 4 dwelling units Availing Premium FSI</t>
-  </si>
-  <si>
-    <t>4 dwelling units</t>
-  </si>
-  <si>
-    <t>Plot No.557, Door No.31, 4th Sector, 14th Street, K.K. Nagar, Chennai 600078 comprised in Old S.No.275/1 (Pt) (Document) and T.S.No.21, Block No.56 of Virugambakkam Village, within the limit of Greater Chennai Corporation</t>
-  </si>
-  <si>
-    <t>Puliyur</t>
-  </si>
-  <si>
-    <t>CMDA/PP/NHRB/C/0935/2024</t>
-  </si>
-  <si>
-    <t>OL-PP/NHRB/0285/2025</t>
-  </si>
-  <si>
-    <t>OL-01981</t>
-  </si>
-  <si>
-    <t>30/12/2024</t>
-  </si>
-  <si>
-    <t>9840312727</t>
-  </si>
-  <si>
-    <t>syeddhasthakir@gmail.com</t>
-  </si>
-  <si>
-    <t>KR YUVITH</t>
-  </si>
-  <si>
-    <t>114, 114, BHASKAR COLONY 3RD STREET, , VIRUGAMBAKKAM, Koyambedu</t>
-  </si>
-  <si>
-    <t>Proposed construction of Stilt Floor + 5 Floors Residential Building (Height-18.00m) with 17 Dwelling Units availing premium FSI with TOD benefit</t>
-  </si>
-  <si>
-    <t>17 Dwelling Units</t>
-  </si>
-  <si>
-    <t>Plot No.56,57 &amp; 58, Door No.30, Old Door No.30(57) &amp; New Door No.17, Elango Nagar Main Road, Virugambakkam, Chennai comprised in Old S.No.146(part) and T.S.No.78 &amp; 79, Block No.5 of Virugambakkam village, Mambalam Taluk within the Limits of Greater Chennai Corporation</t>
+    <t>CMDA/PP/NHRB/N/0239/2025</t>
+  </si>
+  <si>
+    <t>OL-PP/NHRB/0297/2025</t>
+  </si>
+  <si>
+    <t>OL-01996</t>
+  </si>
+  <si>
+    <t>25-07-2025</t>
+  </si>
+  <si>
+    <t>04/04/2025</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+  <si>
+    <t>npsdevelopers.md@gmail.com</t>
+  </si>
+  <si>
+    <t>NPSH Developers Pvt Ltd</t>
+  </si>
+  <si>
+    <t>25, 25, Kattabomman Street, Virugambakkam, Chennai 600092</t>
+  </si>
+  <si>
+    <t>Proposed construction of Stilt Floor (Parking) + 3 Floors Residential Building with 16 dwelling units (Height- 13.20 m)</t>
+  </si>
+  <si>
+    <t>16 dwelling units</t>
+  </si>
+  <si>
+    <t>at Plot No.213, Ranganayaki Ammal Street, Ayyavu Naidu Colony, Arumbakkam, Chennai- 600 029, comprised in Old R.S.No. 46/2pt &amp; 45/6pt and T.S.No. 4/16 &amp; 54, Block No.22 &amp; 23 , Ward.001 of Arumbakkam village, Aminijikarai Taluk Within the limits of Greater Chennai Corporation</t>
+  </si>
+  <si>
+    <t>Arumbakkam</t>
+  </si>
+  <si>
+    <t>CMDA/PP/NHRB/S/0162/2025</t>
+  </si>
+  <si>
+    <t>OL-PP/NHRB/0161/2025</t>
+  </si>
+  <si>
+    <t>OL-01776</t>
+  </si>
+  <si>
+    <t>08-05-2025</t>
+  </si>
+  <si>
+    <t>11/03/2025</t>
+  </si>
+  <si>
+    <t>7550189065</t>
+  </si>
+  <si>
+    <t>ramusundaram1994@gmail.com</t>
+  </si>
+  <si>
+    <t>MS SRISTI REP BY ITS PARTNER MR S RAMUSUNDARAM GPA</t>
+  </si>
+  <si>
+    <t>171/113, NIL, ST.MARY'S ROAD, ABHIRAMAPURAM, CHENNAI 600018, Mylapore</t>
+  </si>
+  <si>
+    <t>Planning Permission for the proposed construction Stilt floor + 4 floors (Height - 17.90m) Residential Building with 6 dwelling units</t>
+  </si>
+  <si>
+    <t>6 dwelling units</t>
+  </si>
+  <si>
+    <t>Plot No.212, 5th Cross Street, Classic Retreat, Shollinganallur, Chennai 600119 comprised in Old S.No.594/3A &amp; 594/4 (pt), New S.No.594/3 of Sholinganallur Village within the limit of Greater Chennai Corporation</t>
+  </si>
+  <si>
+    <t>Sholinganallur</t>
+  </si>
+  <si>
+    <t>CMDA/PP/NHRB/S/0198/2025</t>
+  </si>
+  <si>
+    <t>OL-PP/NHRB/0238/2025</t>
+  </si>
+  <si>
+    <t>OL-01905</t>
+  </si>
+  <si>
+    <t>21/03/2025</t>
+  </si>
+  <si>
+    <t>8428009977</t>
+  </si>
+  <si>
+    <t>office.preethafoundation@gmail.com</t>
+  </si>
+  <si>
+    <t>Ms PREETHA FOUNDATION JANANI CONSTRUCTIONS REP BY ITS PARTNERS Mr SHAKTHI NARAIN C N AND Ms AKSHAYA MOORTHY</t>
+  </si>
+  <si>
+    <t>9/5, NIL, VENKATRAMAN STREET, , PERAMBUR CHENNAI 600011, Okkiam Thorapakkam</t>
+  </si>
+  <si>
+    <t>Proposed construction of Stilt Floor + 3 Floors (Height - 12.80m) Residential Building with 12 Dwelling Units</t>
+  </si>
+  <si>
+    <t>12 Dwelling Units</t>
+  </si>
+  <si>
+    <t>Plot No.22 (CMDA Approved Layout P.P.D/L.O No.6/82), Vetrivelan Nagar, Sithalapakkam, Chennai Comprised in Old S.No.33/1A (Document), S.No.33/12 (Patta) of Sithalapakkam Village within the Limits of St.Thomas Mount Panchayat Union</t>
+  </si>
+  <si>
+    <t>Sithalapakkam</t>
+  </si>
+  <si>
+    <t>CMDA/PP/NHRB/S/0174/2025</t>
+  </si>
+  <si>
+    <t>OL-PP/NHRB/0158/2025</t>
+  </si>
+  <si>
+    <t>OL-01765</t>
+  </si>
+  <si>
+    <t>30-04-2025</t>
+  </si>
+  <si>
+    <t>14/03/2025</t>
+  </si>
+  <si>
+    <t>9840992353</t>
+  </si>
+  <si>
+    <t>vdc.arch@gmail.com</t>
+  </si>
+  <si>
+    <t>Mrs Shashikala Reddy</t>
+  </si>
+  <si>
+    <t>34, Nil, Mudichur Road, West Tambaram, Chennai 600045, Tambaram</t>
+  </si>
+  <si>
+    <t>Planning Permission Application for the proposed construction of Basement floor (TW Parking) + Stilt floor + 4 floors (Height - 17.68m) Commercial cum Residential Building with 1 dwelling (1st to 3rd floor - Office and 4th floor - Residential)</t>
+  </si>
+  <si>
+    <t>1 dwelling</t>
+  </si>
+  <si>
+    <t>Door No.2, Muthulingam Street, Tambaram, Chennai 600045, Comprised in S.No.325/1A1A1A2, 325/1A1A1B &amp; 324/2, and T.S.No.29, 30, 31, 32, 33 &amp; 34, Block No.18, Ward - C of Tambaram Village, Tambaram Taluk within the limit of Tambaram Municipal Corporation</t>
   </si>
   <si>
     <t>Tambaram</t>
-  </si>
-  <si>
-    <t>CMDA/PP/NHRB/C/0650/2024</t>
-  </si>
-  <si>
-    <t>OL-PP/NHRB/0018/2025</t>
-  </si>
-  <si>
-    <t>OL-01520</t>
-  </si>
-  <si>
-    <t>25-01-2025</t>
-  </si>
-  <si>
-    <t>17/09/2024</t>
-  </si>
-  <si>
-    <t>9841055299</t>
-  </si>
-  <si>
-    <t>prasanhousing@gmail.com</t>
-  </si>
-  <si>
-    <t>PRASAN HOUSING REP BY YOKANATHAN AND OTHERS</t>
-  </si>
-  <si>
-    <t>110/62, SHOP 9, TNHB COMPLEX 4TH AVENUE, , ASHOK NAGAR CHENNAI, Thiyagaraya Nagar</t>
-  </si>
-  <si>
-    <t>Proposed Construction of Stilt floor (Parking)+ 5 Floors Residential Building (Height -18.30m ) with 10 Dwelling units , Availing Premium FSI</t>
-  </si>
-  <si>
-    <t>10 Dwelling units</t>
-  </si>
-  <si>
-    <t>Plot/ Door No: 786 Dr.Ramasamy Salai, K.K.Nagar, Chennai .600078, Comprised in Old S.No: 233 part and T.S. No: 373 , Block No: 52 of Virugambakkam Village within the limits of Greater Chennai Corporation</t>
-  </si>
-  <si>
-    <t>Neelangarai</t>
-  </si>
-  <si>
-    <t>CMDA/PP/LAYOUT-1/0031/2025</t>
-  </si>
-  <si>
-    <t>OL-PPD/LO/0080/2025</t>
-  </si>
-  <si>
-    <t>OL-01750</t>
-  </si>
-  <si>
-    <t>28-04-2025</t>
-  </si>
-  <si>
-    <t>05/02/2025</t>
-  </si>
-  <si>
-    <t>Not Found</t>
-  </si>
-  <si>
-    <t>romanticnanda.1972@gmail.com</t>
-  </si>
-  <si>
-    <t>Mr NANDA KUMAR</t>
-  </si>
-  <si>
-    <t>1, 59, NEELAKANDA MUDHALI STREET, VANAGARAM, CHENNAI</t>
-  </si>
-  <si>
-    <t>Planning Permission Application for the proposed Laying out of House Sites in the property</t>
-  </si>
-  <si>
-    <t>S.No.36/6 of Voyalanallur-A Village, Ponamallee Taluk, Thiruvallur District, Poonamallee Panchayat Union Limit</t>
-  </si>
-  <si>
-    <t>Angadu</t>
-  </si>
-  <si>
-    <t>CMDA/PP/LAYOUT-1/0270/2024</t>
-  </si>
-  <si>
-    <t>OL-PPD/LO/0010/2025</t>
-  </si>
-  <si>
-    <t>OL-01507</t>
-  </si>
-  <si>
-    <t>23-01-2025</t>
-  </si>
-  <si>
-    <t>9380553687</t>
-  </si>
-  <si>
-    <t>SHANKARSAMY76@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>G D SATHYANARAYANAN</t>
-  </si>
-  <si>
-    <t>2, 114, ANE ENTERPRISES, VGN NAGAR, AYYAPPANTHANGAL</t>
-  </si>
-  <si>
-    <t>Old S.No.459/1part, T.S.No.55/1 and 55/5, Block No.84, Ward No. I of Paruthipattu Village, Avadi Taluk, Thiruvallur District within the limits of Avadi Corporation</t>
-  </si>
-  <si>
-    <t>Ambathur</t>
-  </si>
-  <si>
-    <t>CMDA/PP/NHRB/S/0617/2024</t>
-  </si>
-  <si>
-    <t>OL-PP/NHRB/0110/2025</t>
-  </si>
-  <si>
-    <t>OL-01673</t>
-  </si>
-  <si>
-    <t>27-03-2025</t>
-  </si>
-  <si>
-    <t>09/09/2024</t>
-  </si>
-  <si>
-    <t>9087872506</t>
-  </si>
-  <si>
-    <t>avittamhomes@gmail.com</t>
-  </si>
-  <si>
-    <t>AVITTAM HOMES Represented by its Proprietor Thiru.D.Sivashanmugam, Avittam Nammalwar,G</t>
-  </si>
-  <si>
-    <t>1 LIC Colony 1st Cross Street, Thiruneermalai Main Road, Pammal, Chennai - 600 075</t>
-  </si>
-  <si>
-    <t>Proposed construction of Residential Group Housing Development with 2 Blocks; Block 1 - Stilt floor + 5 floors (Height - 18.30m) Residential Building with 65 Dwelling; Block 2 - Stilt floor + 5 floors (Height - 18.30m) Residential Building with 50 Dwelling units; Totally 115 Dwelling units for Affordable Housing</t>
-  </si>
-  <si>
-    <t>65 Dwelling</t>
-  </si>
-  <si>
-    <t>Dharkast Road (Kishkindha Main Road), Kannadapalayam, West Tambaram, Chennai 600045, comprised in Old S.Nos.268/2, 268/3 &amp; 268/4, and T.S.Nos.106/1, 107/2, 107/3, 108/2 &amp; 108/3, Block No.21, Ward No.C of Tambaram Village, Tambaram Taluk within the Limits of Tambaram Municipal Corporation</t>
-  </si>
-  <si>
-    <t>9.P.Elanchezhiyan. B.Arch.,M.T.P</t>
-  </si>
-  <si>
-    <t>CMDA Regn. No. RA/Gr.I/19/06/276, No. 14/S2, Thirumurthy Nagar, Madananda puram,, Chennai- 600 125.</t>
-  </si>
-  <si>
-    <t>elan@rspindia.net</t>
   </si>
 </sst>
 </file>
@@ -411,10 +339,16 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -428,6 +362,26 @@
     <font>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -878,156 +832,159 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1374,13 +1331,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="21.6666666666667" customWidth="1"/>
@@ -1405,318 +1362,318 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:20">
-      <c r="A2" t="s">
+    <row r="2" s="1" customFormat="1" ht="15.75" spans="1:20">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:20">
-      <c r="A3" t="s">
+    <row r="3" s="1" customFormat="1" ht="13" customHeight="1" spans="1:20">
+      <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:20">
-      <c r="A4" t="s">
+    <row r="4" s="1" customFormat="1" ht="15.75" spans="1:20">
+      <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:20">
-      <c r="A5" t="s">
+    <row r="5" s="1" customFormat="1" ht="15.75" spans="1:20">
+      <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K5" t="s">
+      <c r="J5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M5" t="s">
+      <c r="L5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="M5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="T5" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="1:20">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" s="2" customFormat="1" ht="15.75" spans="1:20">
+      <c r="A6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1748,180 +1705,21 @@
         <v>96</v>
       </c>
       <c r="K7" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="L7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M7" t="s">
-        <v>98</v>
-      </c>
-      <c r="R7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="R7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="S7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="T7" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" spans="1:20">
-      <c r="A8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I8" t="s">
-        <v>106</v>
-      </c>
-      <c r="J8" t="s">
-        <v>96</v>
-      </c>
-      <c r="K8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L8" t="s">
-        <v>107</v>
-      </c>
-      <c r="M8" t="s">
-        <v>108</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" spans="1:20">
-      <c r="A9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H9" t="s">
-        <v>116</v>
-      </c>
-      <c r="I9" t="s">
-        <v>117</v>
-      </c>
-      <c r="J9" t="s">
-        <v>118</v>
-      </c>
-      <c r="K9" t="s">
-        <v>119</v>
-      </c>
-      <c r="L9" t="s">
-        <v>120</v>
-      </c>
-      <c r="M9" t="s">
-        <v>108</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" customFormat="1" ht="15.75" spans="1:20">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="O10" t="s">
-        <v>122</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T10" s="3" t="s">
+      <c r="T7" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1936,24 +1734,15 @@
     <hyperlink ref="R4" r:id="rId7" display="View PDF"/>
     <hyperlink ref="S4" r:id="rId8" display="View Approved Plan"/>
     <hyperlink ref="T4" r:id="rId9" display="View Approval Letter"/>
-    <hyperlink ref="R5" r:id="rId10" display="View PDF"/>
-    <hyperlink ref="S5" r:id="rId11" display="View Approved Plan"/>
-    <hyperlink ref="T5" r:id="rId12" display="View Approval Letter"/>
-    <hyperlink ref="R6" r:id="rId13" display="View PDF"/>
-    <hyperlink ref="S6" r:id="rId14" display="View Approved Plan"/>
-    <hyperlink ref="T6" r:id="rId15" display="View Approval Letter"/>
+    <hyperlink ref="R6" r:id="rId10" display="View PDF"/>
+    <hyperlink ref="S6" r:id="rId11" display="View Approved Plan"/>
+    <hyperlink ref="T6" r:id="rId12" display="View Approval Letter"/>
+    <hyperlink ref="R5" r:id="rId13" display="View PDF"/>
+    <hyperlink ref="S5" r:id="rId14" display="View Approved Plan"/>
+    <hyperlink ref="T5" r:id="rId15" display="View Approval Letter"/>
     <hyperlink ref="R7" r:id="rId16" display="View PDF"/>
     <hyperlink ref="S7" r:id="rId17" display="View Approved Plan"/>
     <hyperlink ref="T7" r:id="rId18" display="View Approval Letter"/>
-    <hyperlink ref="R8" r:id="rId19" display="View PDF"/>
-    <hyperlink ref="S8" r:id="rId20" display="View Approved Plan"/>
-    <hyperlink ref="T8" r:id="rId21" display="View Approval Letter"/>
-    <hyperlink ref="R9" r:id="rId22" display="View PDF"/>
-    <hyperlink ref="S9" r:id="rId23" display="View Approved Plan"/>
-    <hyperlink ref="T9" r:id="rId24" display="View Approval Letter"/>
-    <hyperlink ref="R10" r:id="rId1" display="View PDF"/>
-    <hyperlink ref="S10" r:id="rId2" display="View Approved Plan"/>
-    <hyperlink ref="T10" r:id="rId3" display="View Approval Letter"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>